<commit_message>
Add mac-addr, software, url targets
</commit_message>
<xml_diff>
--- a/data_gen/openc2_genj.xlsx
+++ b/data_gen/openc2_genj.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="462">
-  <si>
-    <t>Generated from data\openc2.jaen, Fri Mar 10 13:43:58 2017</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="463">
+  <si>
+    <t>Generated from data\openc2.jaen, Fri Mar 10 14:52:35 2017</t>
   </si>
   <si>
     <t>module</t>
@@ -381,7 +381,7 @@
     <t>mac_addr</t>
   </si>
   <si>
-    <t>mac-addr (Record)</t>
+    <t>mac-addr (String)</t>
   </si>
   <si>
     <t>memory</t>
@@ -411,7 +411,7 @@
     <t>url</t>
   </si>
   <si>
-    <t>url (Record)</t>
+    <t>url (String)</t>
   </si>
   <si>
     <t>user_account</t>
@@ -945,6 +945,36 @@
     <t>whirlpool cryptographic hash function as defined in ISO/IEC 10118-3:2004</t>
   </si>
   <si>
+    <t>type (required)</t>
+  </si>
+  <si>
+    <t>MUST be "artifact"</t>
+  </si>
+  <si>
+    <t>mime_type (optional)</t>
+  </si>
+  <si>
+    <t>MUST be a valid MIME type as specified in the IANA Media Types registry</t>
+  </si>
+  <si>
+    <t>* (optional)</t>
+  </si>
+  <si>
+    <t>payload (Choice)</t>
+  </si>
+  <si>
+    <t>choice of literal content or URL to obtain content</t>
+  </si>
+  <si>
+    <t>hashes (optional)</t>
+  </si>
+  <si>
+    <t>hashes-type (Map)</t>
+  </si>
+  <si>
+    <t>Specifies a dictionary of hashes for the contents of the payload</t>
+  </si>
+  <si>
     <t>payload</t>
   </si>
   <si>
@@ -960,36 +990,6 @@
     <t>MUST be a valid URL that resolves to the un-encoded content</t>
   </si>
   <si>
-    <t>type (required)</t>
-  </si>
-  <si>
-    <t>MUST be "artifact"</t>
-  </si>
-  <si>
-    <t>mime_type (optional)</t>
-  </si>
-  <si>
-    <t>MUST be a valid MIME type as specified in the IANA Media Types registry</t>
-  </si>
-  <si>
-    <t>* (optional)</t>
-  </si>
-  <si>
-    <t>payload (Choice)</t>
-  </si>
-  <si>
-    <t>choice of literal content or URL to obtain content</t>
-  </si>
-  <si>
-    <t>hashes (optional)</t>
-  </si>
-  <si>
-    <t>hashes-type (Map)</t>
-  </si>
-  <si>
-    <t>Specifies a dictionary of hashes for the contents of the payload</t>
-  </si>
-  <si>
     <t>Target used to query Actuator for its supported capabilities</t>
   </si>
   <si>
@@ -1146,21 +1146,12 @@
     <t>TODO: finish</t>
   </si>
   <si>
-    <t>ipv4-str</t>
+    <t>ipv4-addr</t>
   </si>
   <si>
     <t>IPv4 address or range in CIDR notation</t>
   </si>
   <si>
-    <t>ipv4-addr</t>
-  </si>
-  <si>
-    <t>ipv4-str (String)</t>
-  </si>
-  <si>
-    <t>Specifies one or more IPv4 addresses</t>
-  </si>
-  <si>
     <t>resolves_to_refs (optional)</t>
   </si>
   <si>
@@ -1179,220 +1170,232 @@
     <t>Specifies a reference to one or more autonomous systems (AS) that the IPv4 address belongs to.</t>
   </si>
   <si>
-    <t>ipv6-str</t>
+    <t>ipv6-addr</t>
   </si>
   <si>
     <t>IPv6 address or range</t>
   </si>
   <si>
-    <t>ipv6-addr</t>
-  </si>
-  <si>
-    <t>ipv6-str (String)</t>
-  </si>
-  <si>
-    <t>Specifies one or more IPv6 addresses</t>
-  </si>
-  <si>
     <t>mac-addrs</t>
   </si>
   <si>
+    <t>mac-addr</t>
+  </si>
+  <si>
+    <t>Colon-delimited MAC-48 address with leading zeros for each octet</t>
+  </si>
+  <si>
     <t>asystems</t>
   </si>
   <si>
     <t>autonomous-system</t>
   </si>
   <si>
-    <t>mac-addr</t>
-  </si>
-  <si>
-    <t>Specifies a single MAC address.  MUST be represented as a single colon-delimited, lowercase MAC-48 address, which MUST include leading zeros for each octet.  Example: 00:00:ab:cd:ef:01</t>
-  </si>
-  <si>
-    <t>mutex</t>
+    <t>ip-connection</t>
+  </si>
+  <si>
+    <t>5-tuple that specifies a tcp/ip connection</t>
+  </si>
+  <si>
+    <t>src_addr (optional)</t>
+  </si>
+  <si>
+    <t>source address</t>
+  </si>
+  <si>
+    <t>src_port (optional)</t>
+  </si>
+  <si>
+    <t>port (Choice)</t>
+  </si>
+  <si>
+    <t>source TCP/UDP port number</t>
+  </si>
+  <si>
+    <t>dst_addr (optional)</t>
+  </si>
+  <si>
+    <t>destination address</t>
+  </si>
+  <si>
+    <t>dst_port (optional)</t>
+  </si>
+  <si>
+    <t>destination TCP/UDP port number</t>
+  </si>
+  <si>
+    <t>layer3_protocol (optional)</t>
+  </si>
+  <si>
+    <t>layer3-protocol (vocab)</t>
+  </si>
+  <si>
+    <t>IEEE 802 Ether Type</t>
+  </si>
+  <si>
+    <t>layer4_protocol (optional)</t>
+  </si>
+  <si>
+    <t>layer4-protocol (vocab)</t>
+  </si>
+  <si>
+    <t>Protocol (IPv4) / Next Header (IPv6)</t>
+  </si>
+  <si>
+    <t>port</t>
+  </si>
+  <si>
+    <t>TCP/UDP port number or protocol</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Port number (e.g., dynamically assigned)</t>
+  </si>
+  <si>
+    <t>protocol</t>
+  </si>
+  <si>
+    <t>layer7-protocol (vocab)</t>
+  </si>
+  <si>
+    <t>Registered port nummber (registered with IANA)</t>
+  </si>
+  <si>
+    <t>layer3-protocol</t>
+  </si>
+  <si>
+    <t>IEEE 802 Ether Types - any IANA value, RFC 7042</t>
+  </si>
+  <si>
+    <t>IPv4</t>
+  </si>
+  <si>
+    <t>0x0800 Internet Protocol Version 4</t>
+  </si>
+  <si>
+    <t>ARP</t>
+  </si>
+  <si>
+    <t>0x0806 Address Resolution Protocol</t>
+  </si>
+  <si>
+    <t>IPv6</t>
+  </si>
+  <si>
+    <t>0x86DD Internet Protocol Version 6</t>
+  </si>
+  <si>
+    <t>MPLS</t>
+  </si>
+  <si>
+    <t>0x8847 Multi-Protocol Label Switching</t>
+  </si>
+  <si>
+    <t>layer4-protocol</t>
+  </si>
+  <si>
+    <t>protocol (IPv4) or next header (IPv6) field - any IANA value, RFC 5237</t>
+  </si>
+  <si>
+    <t>ICMP</t>
+  </si>
+  <si>
+    <t>Internet Control Message Protocol - RFC 792</t>
+  </si>
+  <si>
+    <t>TCP</t>
+  </si>
+  <si>
+    <t>Transmission Control Protocol - RFC 793</t>
+  </si>
+  <si>
+    <t>UDP</t>
+  </si>
+  <si>
+    <t>User Datagram Protocol - RFC 768</t>
+  </si>
+  <si>
+    <t>layer7-protocol</t>
+  </si>
+  <si>
+    <t>Service Name and Transport Protocol Port - any IANA value, RFC 6335</t>
+  </si>
+  <si>
+    <t>ftp-data</t>
+  </si>
+  <si>
+    <t>File Transfer Protocol (data)</t>
+  </si>
+  <si>
+    <t>ftp</t>
+  </si>
+  <si>
+    <t>File Transfer Protocol (control)</t>
+  </si>
+  <si>
+    <t>ssh</t>
+  </si>
+  <si>
+    <t>Secure Shell Protocol</t>
+  </si>
+  <si>
+    <t>telnet</t>
+  </si>
+  <si>
+    <t>Telnet</t>
+  </si>
+  <si>
+    <t>smtp</t>
+  </si>
+  <si>
+    <t>Simple Mail Transfer Protocol</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t>Hypertext Transport Protocol</t>
+  </si>
+  <si>
+    <t>https</t>
+  </si>
+  <si>
+    <t>HTTP over TLS</t>
   </si>
   <si>
     <t>name (required)</t>
   </si>
   <si>
-    <t>Specifies the name of the mutex object.</t>
-  </si>
-  <si>
-    <t>ip-connection</t>
-  </si>
-  <si>
-    <t>5-tuple that specifies a tcp/ip connection</t>
-  </si>
-  <si>
-    <t>src_addr (optional)</t>
-  </si>
-  <si>
-    <t>source address</t>
-  </si>
-  <si>
-    <t>src_port (optional)</t>
-  </si>
-  <si>
-    <t>port (Choice)</t>
-  </si>
-  <si>
-    <t>source TCP/UDP port number</t>
-  </si>
-  <si>
-    <t>dst_addr (optional)</t>
-  </si>
-  <si>
-    <t>destination address</t>
-  </si>
-  <si>
-    <t>dst_port (optional)</t>
-  </si>
-  <si>
-    <t>destination TCP/UDP port number</t>
-  </si>
-  <si>
-    <t>layer3_protocol (optional)</t>
-  </si>
-  <si>
-    <t>layer3-protocol (vocab)</t>
-  </si>
-  <si>
-    <t>IEEE 802 Ether Type</t>
-  </si>
-  <si>
-    <t>layer4_protocol (optional)</t>
-  </si>
-  <si>
-    <t>layer4-protocol (vocab)</t>
-  </si>
-  <si>
-    <t>Protocol (IPv4) / Next Header (IPv6)</t>
-  </si>
-  <si>
-    <t>layer3-protocol</t>
-  </si>
-  <si>
-    <t>IEEE 802 Ether Types - any IANA value, RFC 7042</t>
-  </si>
-  <si>
-    <t>IPv4</t>
-  </si>
-  <si>
-    <t>0x0800 Internet Protocol Version 4</t>
-  </si>
-  <si>
-    <t>ARP</t>
-  </si>
-  <si>
-    <t>0x0806 Address Resolution Protocol</t>
-  </si>
-  <si>
-    <t>IPv6</t>
-  </si>
-  <si>
-    <t>0x86DD Internet Protocol Version 6</t>
-  </si>
-  <si>
-    <t>MPLS</t>
-  </si>
-  <si>
-    <t>0x8847 Multi-Protocol Label Switching</t>
-  </si>
-  <si>
-    <t>port</t>
-  </si>
-  <si>
-    <t>TCP/UDP port number or protocol</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>Port number (e.g., dynamically assigned)</t>
-  </si>
-  <si>
-    <t>protocol</t>
-  </si>
-  <si>
-    <t>layer7-protocol (vocab)</t>
-  </si>
-  <si>
-    <t>Registered port nummber (registered with IANA)</t>
-  </si>
-  <si>
-    <t>layer4-protocol</t>
-  </si>
-  <si>
-    <t>protocol (IPv4) or next header (IPv6) field - any IANA value, RFC 5237</t>
-  </si>
-  <si>
-    <t>ICMP</t>
-  </si>
-  <si>
-    <t>Internet Control Message Protocol - RFC 792</t>
-  </si>
-  <si>
-    <t>TCP</t>
-  </si>
-  <si>
-    <t>Transmission Control Protocol - RFC 793</t>
-  </si>
-  <si>
-    <t>UDP</t>
-  </si>
-  <si>
-    <t>User Datagram Protocol - RFC 768</t>
-  </si>
-  <si>
-    <t>layer7-protocol</t>
-  </si>
-  <si>
-    <t>Service Name and Transport Protocol Port - any IANA value, RFC 6335</t>
-  </si>
-  <si>
-    <t>ftp-data</t>
-  </si>
-  <si>
-    <t>File Transfer Protocol (data)</t>
-  </si>
-  <si>
-    <t>ftp</t>
-  </si>
-  <si>
-    <t>File Transfer Protocol (control)</t>
-  </si>
-  <si>
-    <t>ssh</t>
-  </si>
-  <si>
-    <t>Secure Shell Protocol</t>
-  </si>
-  <si>
-    <t>telnet</t>
-  </si>
-  <si>
-    <t>Telnet</t>
-  </si>
-  <si>
-    <t>smtp</t>
-  </si>
-  <si>
-    <t>Simple Mail Transfer Protocol</t>
-  </si>
-  <si>
-    <t>http</t>
-  </si>
-  <si>
-    <t>Hypertext Transport Protocol</t>
-  </si>
-  <si>
-    <t>https</t>
-  </si>
-  <si>
-    <t>HTTP over TLS</t>
+    <t>Name of the software</t>
+  </si>
+  <si>
+    <t>cpe (optional)</t>
+  </si>
+  <si>
+    <t>From Common Platform Enumeration (CPE) v2.3 dictionary</t>
+  </si>
+  <si>
+    <t>language (optional)</t>
+  </si>
+  <si>
+    <t>Language of the software from ISO 639-2</t>
+  </si>
+  <si>
+    <t>vendor (optional)</t>
+  </si>
+  <si>
+    <t>Vendor of the software</t>
+  </si>
+  <si>
+    <t>version (optional)</t>
+  </si>
+  <si>
+    <t>Version of the software</t>
   </si>
   <si>
     <t>user-account</t>
@@ -1885,7 +1888,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E422"/>
+  <dimension ref="A2:E406"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3978,7 +3981,7 @@
         <v>15</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>309</v>
+        <v>94</v>
       </c>
       <c r="C213" s="5"/>
       <c r="D213" s="5"/>
@@ -3989,7 +3992,7 @@
         <v>16</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C214" s="6"/>
       <c r="D214" s="6"/>
@@ -4014,13 +4017,13 @@
         <v>1</v>
       </c>
       <c r="C217" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="D217" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E217" s="8" t="s">
         <v>310</v>
-      </c>
-      <c r="D217" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E217" s="8" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -4028,102 +4031,102 @@
         <v>2</v>
       </c>
       <c r="C218" s="8" t="s">
-        <v>130</v>
+        <v>311</v>
       </c>
       <c r="D218" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E218" s="8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
+      <c r="B219" s="8">
+        <v>3</v>
+      </c>
+      <c r="C219" s="8" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="221" spans="1:5">
-      <c r="A221" s="4" t="s">
+      <c r="D219" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="E219" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="B220" s="8">
+        <v>4</v>
+      </c>
+      <c r="C220" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D220" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="E220" s="8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5">
+      <c r="A223" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B221" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C221" s="5"/>
-      <c r="D221" s="5"/>
-      <c r="E221" s="5"/>
-    </row>
-    <row r="222" spans="1:5">
-      <c r="A222" s="4" t="s">
+      <c r="B223" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C223" s="5"/>
+      <c r="D223" s="5"/>
+      <c r="E223" s="5"/>
+    </row>
+    <row r="224" spans="1:5">
+      <c r="A224" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B222" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C222" s="6"/>
-      <c r="D222" s="6"/>
-      <c r="E222" s="6"/>
-    </row>
-    <row r="224" spans="1:5">
-      <c r="B224" s="7" t="s">
+      <c r="B224" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C224" s="6"/>
+      <c r="D224" s="6"/>
+      <c r="E224" s="6"/>
+    </row>
+    <row r="226" spans="1:5">
+      <c r="B226" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C224" s="7" t="s">
+      <c r="C226" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D224" s="7" t="s">
+      <c r="D226" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E224" s="7" t="s">
+      <c r="E226" s="7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5">
-      <c r="B225" s="8">
-        <v>1</v>
-      </c>
-      <c r="C225" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="D225" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E225" s="8" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5">
-      <c r="B226" s="8">
-        <v>2</v>
-      </c>
-      <c r="C226" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="D226" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E226" s="8" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="227" spans="1:5">
       <c r="B227" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C227" s="8" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D227" s="8" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E227" s="8" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="228" spans="1:5">
       <c r="B228" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C228" s="8" t="s">
-        <v>321</v>
+        <v>130</v>
       </c>
       <c r="D228" s="8" t="s">
-        <v>322</v>
+        <v>49</v>
       </c>
       <c r="E228" s="8" t="s">
         <v>323</v>
@@ -4828,218 +4831,217 @@
         <v>16</v>
       </c>
       <c r="B316" s="6" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C316" s="6"/>
       <c r="D316" s="6"/>
       <c r="E316" s="6"/>
     </row>
-    <row r="317" spans="1:5">
-      <c r="A317" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B317" s="6" t="s">
+    <row r="318" spans="1:5">
+      <c r="B318" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C318" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D318" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E318" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5">
+      <c r="B319" s="8">
+        <v>1</v>
+      </c>
+      <c r="C319" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="D319" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E319" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="C317" s="6"/>
-      <c r="D317" s="6"/>
-      <c r="E317" s="6"/>
     </row>
     <row r="320" spans="1:5">
-      <c r="A320" s="4" t="s">
+      <c r="B320" s="8">
+        <v>2</v>
+      </c>
+      <c r="C320" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="D320" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="E320" s="8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5">
+      <c r="B321" s="8">
+        <v>3</v>
+      </c>
+      <c r="C321" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="D321" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="E321" s="8" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5">
+      <c r="A324" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B320" s="5" t="s">
+      <c r="B324" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="C324" s="5"/>
+      <c r="D324" s="5"/>
+      <c r="E324" s="5"/>
+    </row>
+    <row r="325" spans="1:5">
+      <c r="A325" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B325" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C325" s="6"/>
+      <c r="D325" s="6"/>
+      <c r="E325" s="6"/>
+    </row>
+    <row r="327" spans="1:5">
+      <c r="B327" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C327" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D327" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E327" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5">
+      <c r="B328" s="8">
+        <v>1</v>
+      </c>
+      <c r="C328" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="D328" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E328" s="8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5">
+      <c r="B329" s="8">
+        <v>2</v>
+      </c>
+      <c r="C329" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="C320" s="5"/>
-      <c r="D320" s="5"/>
-      <c r="E320" s="5"/>
-    </row>
-    <row r="321" spans="1:5">
-      <c r="A321" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B321" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C321" s="6"/>
-      <c r="D321" s="6"/>
-      <c r="E321" s="6"/>
-    </row>
-    <row r="323" spans="1:5">
-      <c r="B323" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C323" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D323" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E323" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="324" spans="1:5">
-      <c r="B324" s="8">
-        <v>1</v>
-      </c>
-      <c r="C324" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="D324" s="8" t="s">
+      <c r="D329" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="E324" s="8" t="s">
+      <c r="E329" s="8" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="325" spans="1:5">
-      <c r="B325" s="8">
-        <v>2</v>
-      </c>
-      <c r="C325" s="8" t="s">
+    <row r="330" spans="1:5">
+      <c r="B330" s="8">
+        <v>3</v>
+      </c>
+      <c r="C330" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="D325" s="8" t="s">
+      <c r="D330" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="E325" s="8" t="s">
+      <c r="E330" s="8" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="326" spans="1:5">
-      <c r="B326" s="8">
-        <v>3</v>
-      </c>
-      <c r="C326" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="D326" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="E326" s="8" t="s">
+    <row r="333" spans="1:5">
+      <c r="A333" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B333" s="5" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="329" spans="1:5">
-      <c r="A329" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B329" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="C329" s="5"/>
-      <c r="D329" s="5"/>
-      <c r="E329" s="5"/>
-    </row>
-    <row r="330" spans="1:5">
-      <c r="A330" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B330" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C330" s="6"/>
-      <c r="D330" s="6"/>
-      <c r="E330" s="6"/>
-    </row>
-    <row r="331" spans="1:5">
-      <c r="A331" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B331" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="C331" s="6"/>
-      <c r="D331" s="6"/>
-      <c r="E331" s="6"/>
+      <c r="C333" s="5"/>
+      <c r="D333" s="5"/>
+      <c r="E333" s="5"/>
     </row>
     <row r="334" spans="1:5">
       <c r="A334" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B334" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="C334" s="6"/>
+      <c r="D334" s="6"/>
+      <c r="E334" s="6"/>
+    </row>
+    <row r="335" spans="1:5">
+      <c r="B335" s="8">
+        <v>0</v>
+      </c>
+      <c r="C335" s="8"/>
+      <c r="D335" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E335" s="8"/>
+    </row>
+    <row r="338" spans="1:5">
+      <c r="A338" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B334" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="C334" s="5"/>
-      <c r="D334" s="5"/>
-      <c r="E334" s="5"/>
-    </row>
-    <row r="335" spans="1:5">
-      <c r="A335" s="4" t="s">
+      <c r="B338" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="C338" s="5"/>
+      <c r="D338" s="5"/>
+      <c r="E338" s="5"/>
+    </row>
+    <row r="339" spans="1:5">
+      <c r="A339" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B335" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C335" s="6"/>
-      <c r="D335" s="6"/>
-      <c r="E335" s="6"/>
-    </row>
-    <row r="337" spans="1:5">
-      <c r="B337" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C337" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D337" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E337" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="338" spans="1:5">
-      <c r="B338" s="8">
-        <v>1</v>
-      </c>
-      <c r="C338" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="D338" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="E338" s="8" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="339" spans="1:5">
-      <c r="B339" s="8">
-        <v>2</v>
-      </c>
-      <c r="C339" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="D339" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E339" s="8" t="s">
-        <v>383</v>
-      </c>
+      <c r="B339" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C339" s="6"/>
+      <c r="D339" s="6"/>
+      <c r="E339" s="6"/>
     </row>
     <row r="340" spans="1:5">
-      <c r="B340" s="8">
-        <v>3</v>
-      </c>
-      <c r="C340" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="D340" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="E340" s="8" t="s">
-        <v>386</v>
-      </c>
+      <c r="A340" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B340" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C340" s="6"/>
+      <c r="D340" s="6"/>
+      <c r="E340" s="6"/>
     </row>
     <row r="343" spans="1:5">
       <c r="A343" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B343" s="5" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C343" s="5"/>
       <c r="D343" s="5"/>
@@ -5062,7 +5064,7 @@
       </c>
       <c r="C345" s="8"/>
       <c r="D345" s="8" t="s">
-        <v>121</v>
+        <v>390</v>
       </c>
       <c r="E345" s="8"/>
     </row>
@@ -5071,7 +5073,7 @@
         <v>15</v>
       </c>
       <c r="B348" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C348" s="5"/>
       <c r="D348" s="5"/>
@@ -5082,546 +5084,470 @@
         <v>16</v>
       </c>
       <c r="B349" s="6" t="s">
-        <v>351</v>
+        <v>29</v>
       </c>
       <c r="C349" s="6"/>
       <c r="D349" s="6"/>
       <c r="E349" s="6"/>
     </row>
     <row r="350" spans="1:5">
-      <c r="B350" s="8">
-        <v>0</v>
-      </c>
-      <c r="C350" s="8"/>
-      <c r="D350" s="8" t="s">
+      <c r="A350" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B350" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="C350" s="6"/>
+      <c r="D350" s="6"/>
+      <c r="E350" s="6"/>
+    </row>
+    <row r="352" spans="1:5">
+      <c r="B352" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C352" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D352" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E352" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5">
+      <c r="B353" s="8">
+        <v>1</v>
+      </c>
+      <c r="C353" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="D353" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="E353" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="E350" s="8"/>
-    </row>
-    <row r="353" spans="1:5">
-      <c r="A353" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B353" s="5" t="s">
+    </row>
+    <row r="354" spans="1:5">
+      <c r="B354" s="8">
+        <v>2</v>
+      </c>
+      <c r="C354" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="C353" s="5"/>
-      <c r="D353" s="5"/>
-      <c r="E353" s="5"/>
-    </row>
-    <row r="354" spans="1:5">
-      <c r="A354" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B354" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C354" s="6"/>
-      <c r="D354" s="6"/>
-      <c r="E354" s="6"/>
+      <c r="D354" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E354" s="8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5">
+      <c r="B355" s="8">
+        <v>3</v>
+      </c>
+      <c r="C355" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D355" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="E355" s="8" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="356" spans="1:5">
-      <c r="B356" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C356" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D356" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E356" s="7" t="s">
-        <v>21</v>
+      <c r="B356" s="8">
+        <v>4</v>
+      </c>
+      <c r="C356" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D356" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E356" s="8" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="357" spans="1:5">
       <c r="B357" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C357" s="8" t="s">
-        <v>357</v>
+        <v>402</v>
       </c>
       <c r="D357" s="8" t="s">
-        <v>49</v>
+        <v>403</v>
       </c>
       <c r="E357" s="8" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="360" spans="1:5">
-      <c r="A360" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B360" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="C360" s="5"/>
-      <c r="D360" s="5"/>
-      <c r="E360" s="5"/>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5">
+      <c r="B358" s="8">
+        <v>6</v>
+      </c>
+      <c r="C358" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="D358" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="E358" s="8" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="361" spans="1:5">
       <c r="A361" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B361" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="C361" s="5"/>
+      <c r="D361" s="5"/>
+      <c r="E361" s="5"/>
+    </row>
+    <row r="362" spans="1:5">
+      <c r="A362" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B361" s="6" t="s">
+      <c r="B362" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C362" s="6"/>
+      <c r="D362" s="6"/>
+      <c r="E362" s="6"/>
+    </row>
+    <row r="363" spans="1:5">
+      <c r="A363" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B363" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="C363" s="6"/>
+      <c r="D363" s="6"/>
+      <c r="E363" s="6"/>
+    </row>
+    <row r="365" spans="1:5">
+      <c r="B365" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C365" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D365" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E365" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5">
+      <c r="B366" s="8">
+        <v>1</v>
+      </c>
+      <c r="C366" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="D366" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="E366" s="8" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5">
+      <c r="B367" s="8">
+        <v>2</v>
+      </c>
+      <c r="C367" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="D367" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="E367" s="8" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="370" spans="1:5">
+      <c r="A370" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B370" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C370" s="5"/>
+      <c r="D370" s="5"/>
+      <c r="E370" s="5"/>
+    </row>
+    <row r="371" spans="1:5">
+      <c r="A371" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B371" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C361" s="6"/>
-      <c r="D361" s="6"/>
-      <c r="E361" s="6"/>
-    </row>
-    <row r="363" spans="1:5">
-      <c r="B363" s="7" t="s">
+      <c r="C371" s="6"/>
+      <c r="D371" s="6"/>
+      <c r="E371" s="6"/>
+    </row>
+    <row r="373" spans="1:5">
+      <c r="B373" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C363" s="7" t="s">
+      <c r="C373" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D363" s="7" t="s">
+      <c r="D373" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E363" s="7" t="s">
+      <c r="E373" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="364" spans="1:5">
-      <c r="B364" s="8">
+    <row r="376" spans="1:5">
+      <c r="A376" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B376" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C376" s="5"/>
+      <c r="D376" s="5"/>
+      <c r="E376" s="5"/>
+    </row>
+    <row r="377" spans="1:5">
+      <c r="A377" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B377" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C377" s="6"/>
+      <c r="D377" s="6"/>
+      <c r="E377" s="6"/>
+    </row>
+    <row r="379" spans="1:5">
+      <c r="B379" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C379" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D379" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E379" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="380" spans="1:5">
+      <c r="B380" s="8">
         <v>1</v>
       </c>
-      <c r="C364" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="D364" s="8" t="s">
+      <c r="C380" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="D380" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E364" s="8" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="367" spans="1:5">
-      <c r="A367" s="4" t="s">
+      <c r="E380" s="8" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="381" spans="1:5">
+      <c r="B381" s="8">
+        <v>2</v>
+      </c>
+      <c r="C381" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="D381" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E381" s="8" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="382" spans="1:5">
+      <c r="B382" s="8">
+        <v>3</v>
+      </c>
+      <c r="C382" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="D382" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E382" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="383" spans="1:5">
+      <c r="B383" s="8">
+        <v>4</v>
+      </c>
+      <c r="C383" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="D383" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E383" s="8" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="384" spans="1:5">
+      <c r="B384" s="8">
+        <v>5</v>
+      </c>
+      <c r="C384" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="D384" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E384" s="8" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5">
+      <c r="A387" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B367" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="C367" s="5"/>
-      <c r="D367" s="5"/>
-      <c r="E367" s="5"/>
-    </row>
-    <row r="368" spans="1:5">
-      <c r="A368" s="4" t="s">
+      <c r="B387" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C387" s="5"/>
+      <c r="D387" s="5"/>
+      <c r="E387" s="5"/>
+    </row>
+    <row r="388" spans="1:5">
+      <c r="A388" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B368" s="6" t="s">
+      <c r="B388" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C388" s="6"/>
+      <c r="D388" s="6"/>
+      <c r="E388" s="6"/>
+    </row>
+    <row r="391" spans="1:5">
+      <c r="A391" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B391" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="C391" s="5"/>
+      <c r="D391" s="5"/>
+      <c r="E391" s="5"/>
+    </row>
+    <row r="392" spans="1:5">
+      <c r="A392" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B392" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C368" s="6"/>
-      <c r="D368" s="6"/>
-      <c r="E368" s="6"/>
-    </row>
-    <row r="369" spans="1:5">
-      <c r="A369" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B369" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="C369" s="6"/>
-      <c r="D369" s="6"/>
-      <c r="E369" s="6"/>
-    </row>
-    <row r="371" spans="1:5">
-      <c r="B371" s="7" t="s">
+      <c r="C392" s="6"/>
+      <c r="D392" s="6"/>
+      <c r="E392" s="6"/>
+    </row>
+    <row r="394" spans="1:5">
+      <c r="B394" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C371" s="7" t="s">
+      <c r="C394" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D371" s="7" t="s">
+      <c r="D394" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E371" s="7" t="s">
+      <c r="E394" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="372" spans="1:5">
-      <c r="B372" s="8">
-        <v>1</v>
-      </c>
-      <c r="C372" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="D372" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="E372" s="8" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="373" spans="1:5">
-      <c r="B373" s="8">
-        <v>2</v>
-      </c>
-      <c r="C373" s="8" t="s">
-        <v>404</v>
-      </c>
-      <c r="D373" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="E373" s="8" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="374" spans="1:5">
-      <c r="B374" s="8">
-        <v>3</v>
-      </c>
-      <c r="C374" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="D374" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="E374" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="375" spans="1:5">
-      <c r="B375" s="8">
-        <v>4</v>
-      </c>
-      <c r="C375" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="D375" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="E375" s="8" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="376" spans="1:5">
-      <c r="B376" s="8">
-        <v>5</v>
-      </c>
-      <c r="C376" s="8" t="s">
-        <v>411</v>
-      </c>
-      <c r="D376" s="8" t="s">
-        <v>412</v>
-      </c>
-      <c r="E376" s="8" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="377" spans="1:5">
-      <c r="B377" s="8">
-        <v>6</v>
-      </c>
-      <c r="C377" s="8" t="s">
-        <v>414</v>
-      </c>
-      <c r="D377" s="8" t="s">
-        <v>415</v>
-      </c>
-      <c r="E377" s="8" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="380" spans="1:5">
-      <c r="A380" s="4" t="s">
+    <row r="397" spans="1:5">
+      <c r="A397" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B380" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="C380" s="5"/>
-      <c r="D380" s="5"/>
-      <c r="E380" s="5"/>
-    </row>
-    <row r="381" spans="1:5">
-      <c r="A381" s="4" t="s">
+      <c r="B397" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="C397" s="5"/>
+      <c r="D397" s="5"/>
+      <c r="E397" s="5"/>
+    </row>
+    <row r="398" spans="1:5">
+      <c r="A398" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B381" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C381" s="6"/>
-      <c r="D381" s="6"/>
-      <c r="E381" s="6"/>
-    </row>
-    <row r="382" spans="1:5">
-      <c r="A382" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B382" s="6" t="s">
-        <v>428</v>
-      </c>
-      <c r="C382" s="6"/>
-      <c r="D382" s="6"/>
-      <c r="E382" s="6"/>
-    </row>
-    <row r="384" spans="1:5">
-      <c r="B384" s="7" t="s">
+      <c r="B398" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C398" s="6"/>
+      <c r="D398" s="6"/>
+      <c r="E398" s="6"/>
+    </row>
+    <row r="400" spans="1:5">
+      <c r="B400" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C384" s="7" t="s">
+      <c r="C400" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D384" s="7" t="s">
+      <c r="D400" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E384" s="7" t="s">
+      <c r="E400" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="385" spans="1:5">
-      <c r="B385" s="8">
-        <v>1</v>
-      </c>
-      <c r="C385" s="8" t="s">
-        <v>429</v>
-      </c>
-      <c r="D385" s="8" t="s">
-        <v>430</v>
-      </c>
-      <c r="E385" s="8" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="386" spans="1:5">
-      <c r="B386" s="8">
-        <v>2</v>
-      </c>
-      <c r="C386" s="8" t="s">
-        <v>432</v>
-      </c>
-      <c r="D386" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="E386" s="8" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="389" spans="1:5">
-      <c r="A389" s="4" t="s">
+    <row r="403" spans="1:5">
+      <c r="A403" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B389" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C389" s="5"/>
-      <c r="D389" s="5"/>
-      <c r="E389" s="5"/>
-    </row>
-    <row r="390" spans="1:5">
-      <c r="A390" s="4" t="s">
+      <c r="B403" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="C403" s="5"/>
+      <c r="D403" s="5"/>
+      <c r="E403" s="5"/>
+    </row>
+    <row r="404" spans="1:5">
+      <c r="A404" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B390" s="6" t="s">
+      <c r="B404" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C390" s="6"/>
-      <c r="D390" s="6"/>
-      <c r="E390" s="6"/>
-    </row>
-    <row r="392" spans="1:5">
-      <c r="B392" s="7" t="s">
+      <c r="C404" s="6"/>
+      <c r="D404" s="6"/>
+      <c r="E404" s="6"/>
+    </row>
+    <row r="406" spans="1:5">
+      <c r="B406" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C392" s="7" t="s">
+      <c r="C406" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D392" s="7" t="s">
+      <c r="D406" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E392" s="7" t="s">
+      <c r="E406" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="395" spans="1:5">
-      <c r="A395" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B395" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C395" s="5"/>
-      <c r="D395" s="5"/>
-      <c r="E395" s="5"/>
-    </row>
-    <row r="396" spans="1:5">
-      <c r="A396" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B396" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C396" s="6"/>
-      <c r="D396" s="6"/>
-      <c r="E396" s="6"/>
-    </row>
-    <row r="398" spans="1:5">
-      <c r="B398" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C398" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D398" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E398" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="401" spans="1:5">
-      <c r="A401" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B401" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C401" s="5"/>
-      <c r="D401" s="5"/>
-      <c r="E401" s="5"/>
-    </row>
-    <row r="402" spans="1:5">
-      <c r="A402" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B402" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C402" s="6"/>
-      <c r="D402" s="6"/>
-      <c r="E402" s="6"/>
-    </row>
-    <row r="404" spans="1:5">
-      <c r="B404" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C404" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D404" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E404" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="407" spans="1:5">
-      <c r="A407" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B407" s="5" t="s">
-        <v>459</v>
-      </c>
-      <c r="C407" s="5"/>
-      <c r="D407" s="5"/>
-      <c r="E407" s="5"/>
-    </row>
-    <row r="408" spans="1:5">
-      <c r="A408" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B408" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C408" s="6"/>
-      <c r="D408" s="6"/>
-      <c r="E408" s="6"/>
-    </row>
-    <row r="410" spans="1:5">
-      <c r="B410" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C410" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D410" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E410" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="413" spans="1:5">
-      <c r="A413" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B413" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="C413" s="5"/>
-      <c r="D413" s="5"/>
-      <c r="E413" s="5"/>
-    </row>
-    <row r="414" spans="1:5">
-      <c r="A414" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B414" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C414" s="6"/>
-      <c r="D414" s="6"/>
-      <c r="E414" s="6"/>
-    </row>
-    <row r="416" spans="1:5">
-      <c r="B416" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C416" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D416" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E416" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="419" spans="1:5">
-      <c r="A419" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B419" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="C419" s="5"/>
-      <c r="D419" s="5"/>
-      <c r="E419" s="5"/>
-    </row>
-    <row r="420" spans="1:5">
-      <c r="A420" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B420" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C420" s="6"/>
-      <c r="D420" s="6"/>
-      <c r="E420" s="6"/>
-    </row>
-    <row r="422" spans="1:5">
-      <c r="B422" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C422" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D422" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E422" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="106">
+  <mergeCells count="99">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B11:E11"/>
@@ -5667,8 +5593,8 @@
     <mergeCell ref="B194:E194"/>
     <mergeCell ref="B213:E213"/>
     <mergeCell ref="B214:E214"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="B224:E224"/>
     <mergeCell ref="B231:E231"/>
     <mergeCell ref="B232:E232"/>
     <mergeCell ref="B244:E244"/>
@@ -5694,40 +5620,33 @@
     <mergeCell ref="B310:E310"/>
     <mergeCell ref="B315:E315"/>
     <mergeCell ref="B316:E316"/>
-    <mergeCell ref="B317:E317"/>
-    <mergeCell ref="B320:E320"/>
-    <mergeCell ref="B321:E321"/>
-    <mergeCell ref="B329:E329"/>
-    <mergeCell ref="B330:E330"/>
-    <mergeCell ref="B331:E331"/>
+    <mergeCell ref="B324:E324"/>
+    <mergeCell ref="B325:E325"/>
+    <mergeCell ref="B333:E333"/>
     <mergeCell ref="B334:E334"/>
-    <mergeCell ref="B335:E335"/>
+    <mergeCell ref="B338:E338"/>
+    <mergeCell ref="B339:E339"/>
+    <mergeCell ref="B340:E340"/>
     <mergeCell ref="B343:E343"/>
     <mergeCell ref="B344:E344"/>
     <mergeCell ref="B348:E348"/>
     <mergeCell ref="B349:E349"/>
-    <mergeCell ref="B353:E353"/>
-    <mergeCell ref="B354:E354"/>
-    <mergeCell ref="B360:E360"/>
+    <mergeCell ref="B350:E350"/>
     <mergeCell ref="B361:E361"/>
-    <mergeCell ref="B367:E367"/>
-    <mergeCell ref="B368:E368"/>
-    <mergeCell ref="B369:E369"/>
-    <mergeCell ref="B380:E380"/>
-    <mergeCell ref="B381:E381"/>
-    <mergeCell ref="B382:E382"/>
-    <mergeCell ref="B389:E389"/>
-    <mergeCell ref="B390:E390"/>
-    <mergeCell ref="B395:E395"/>
-    <mergeCell ref="B396:E396"/>
-    <mergeCell ref="B401:E401"/>
-    <mergeCell ref="B402:E402"/>
-    <mergeCell ref="B407:E407"/>
-    <mergeCell ref="B408:E408"/>
-    <mergeCell ref="B413:E413"/>
-    <mergeCell ref="B414:E414"/>
-    <mergeCell ref="B419:E419"/>
-    <mergeCell ref="B420:E420"/>
+    <mergeCell ref="B362:E362"/>
+    <mergeCell ref="B363:E363"/>
+    <mergeCell ref="B370:E370"/>
+    <mergeCell ref="B371:E371"/>
+    <mergeCell ref="B376:E376"/>
+    <mergeCell ref="B377:E377"/>
+    <mergeCell ref="B387:E387"/>
+    <mergeCell ref="B388:E388"/>
+    <mergeCell ref="B391:E391"/>
+    <mergeCell ref="B392:E392"/>
+    <mergeCell ref="B397:E397"/>
+    <mergeCell ref="B398:E398"/>
+    <mergeCell ref="B403:E403"/>
+    <mergeCell ref="B404:E404"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6584,7 +6503,7 @@
         <v>55</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
@@ -6594,7 +6513,7 @@
         <v>92</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
@@ -6615,10 +6534,10 @@
         <v>2048</v>
       </c>
       <c r="C115" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="D115" s="8" t="s">
         <v>419</v>
-      </c>
-      <c r="D115" s="8" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -6626,10 +6545,10 @@
         <v>2054</v>
       </c>
       <c r="C116" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="D116" s="8" t="s">
         <v>421</v>
-      </c>
-      <c r="D116" s="8" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -6637,10 +6556,10 @@
         <v>34525</v>
       </c>
       <c r="C117" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="D117" s="8" t="s">
         <v>423</v>
-      </c>
-      <c r="D117" s="8" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -6648,10 +6567,10 @@
         <v>34887</v>
       </c>
       <c r="C118" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="D118" s="8" t="s">
         <v>425</v>
-      </c>
-      <c r="D118" s="8" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -6659,7 +6578,7 @@
         <v>55</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
@@ -6669,7 +6588,7 @@
         <v>92</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="C121" s="6"/>
       <c r="D121" s="6"/>
@@ -6690,10 +6609,10 @@
         <v>1</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -6701,10 +6620,10 @@
         <v>6</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -6712,10 +6631,10 @@
         <v>17</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -6723,7 +6642,7 @@
         <v>55</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
@@ -6733,7 +6652,7 @@
         <v>92</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="C129" s="6"/>
       <c r="D129" s="6"/>
@@ -6754,10 +6673,10 @@
         <v>20</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -6765,10 +6684,10 @@
         <v>21</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -6776,10 +6695,10 @@
         <v>22</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -6787,10 +6706,10 @@
         <v>23</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -6798,10 +6717,10 @@
         <v>25</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -6809,10 +6728,10 @@
         <v>80</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -6820,10 +6739,10 @@
         <v>443</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>